<commit_message>
Bhaskar - CR 7.2 Financial batches should run more securely
</commit_message>
<xml_diff>
--- a/Development/Artifacts/Changes from CR Mar 2017.xlsx
+++ b/Development/Artifacts/Changes from CR Mar 2017.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Bugzilla Ticket No</t>
   </si>
@@ -57,26 +57,6 @@
   </si>
   <si>
     <t>Bhaskar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('CaseSuspendReason', 'CSR17002', 'Certification Expired', '', '', '1', 0, 'en', CURRENT TIMESTAMP, 1);
-INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('CaseCloseReason', 'CC17007', 'Certification Expired', '', '', '1', 0, 'en', CURRENT TIMESTAMP, 1);
-INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('BatchProcessChunkName', 'BPN17007', 'MOLSA Expired Certification Suspend Case Batch', '', '', '1', 1, 'en', CURRENT TIMESTAMP, 1);
-INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('BatchProcessChunkName', 'BPN17008', 'MOLSA Expired Certification Close Case Batch', '', '', '1', 1, 'en', CURRENT TIMESTAMP, 1);
-INSERT INTO CodeTableHeader (TableName, TimeEntered, DefaultCode, LASTWRITTEN, VERSIONNO) VALUES ('MOLSACertPeriodCode', CURRENT TIMESTAMP, 'CPC17003', CURRENT TIMESTAMP, 1);
-INSERT INTO CTDISPLAYNAME (TableName, LOCALEIdentifier,TEXT,LASTWRITTEN ) VALUES ( 'MOLSACertPeriodCode','en','Certification Period Code', CURRENT TIMESTAMP);
-INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('MOLSACertPeriodCode', 'CPC17003', 'Three Months', '', '', '1', 0, 'en', CURRENT TIMESTAMP, 1);
-INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('MOLSACertPeriodCode', 'CPC17006', 'Six Months', '', '', '1', 0, 'en', CURRENT TIMESTAMP, 1);
-INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('MOLSACertPeriodCode', 'CPC17012', 'Twelve Months', '', '', '1', 0, 'en', CURRENT TIMESTAMP, 1);
-INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSACalcCertDateRange.calcCertificationDates', 'curam', 'molsa.pd.facade', 'curam.molsa.pd.facade.MOLSACalcCertDateRange.calcCertificationDates', 'Y');
-INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSACalcCertDateRange.getCertModifiableInd', 'curam', 'molsa.pd.facade', ' curam.molsa.pd.facade.MOLSACalcCertDateRange.getCertModifiableInd', 'Y');
-INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSACalcCertDateRange.calcCertificationDates', 'FUNCTION', 0);
-INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSACalcCertDateRange.getCertModifiableInd', 'FUNCTION', 0);
-INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSACalcCertDateRange.calcCertificationDates', 'MOLSACalcCertDateRange.calcCertificationDates');
-INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSACalcCertDateRange.getCertModifiableInd', 'MOLSACalcCertDateRange.getCertModifiableInd');
-INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSACalcCertDateRange.calcCertificationDates');
-INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSACalcCertDateRange.getCertModifiableInd');
-</t>
   </si>
   <si>
     <t xml:space="preserve">New Files Added
@@ -127,6 +107,180 @@
 Note: New entry is added and modified existing entry in applicattion.prx file, require build insertproperties
 New javascript is added.
 Navigation file is added that required build inserettabconfiguration</t>
+  </si>
+  <si>
+    <t>INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('CaseSuspendReason', 'CSR17002', 'Certification Expired', '', '', '1', 0, 'en', CURRENT TIMESTAMP, 1);
+INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('CaseCloseReason', 'CC17007', 'Certification Expired', '', '', '1', 0, 'en', CURRENT TIMESTAMP, 1);
+INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('BatchProcessChunkName', 'BPN17007', 'MOLSA Expired Certification Suspend Case Batch', '', '', '1', 1, 'en', CURRENT TIMESTAMP, 1);
+INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('BatchProcessChunkName', 'BPN17008', 'MOLSA Expired Certification Close Case Batch', '', '', '1', 1, 'en', CURRENT TIMESTAMP, 1);
+INSERT INTO CodeTableHeader (TableName, TimeEntered, DefaultCode, LASTWRITTEN, VERSIONNO) VALUES ('MOLSACertPeriodCode', CURRENT TIMESTAMP, 'CPC17003', CURRENT TIMESTAMP, 1);
+INSERT INTO CTDISPLAYNAME (TableName, LOCALEIdentifier,TEXT,LASTWRITTEN ) VALUES ( 'MOLSACertPeriodCode','en','Certification Period Code', CURRENT TIMESTAMP);
+INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('MOLSACertPeriodCode', 'CPC17003', 'Three Months', '', '', '1', 0, 'en', CURRENT TIMESTAMP, 1);
+INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('MOLSACertPeriodCode', 'CPC17006', 'Six Months', '', '', '1', 0, 'en', CURRENT TIMESTAMP, 1);
+INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('MOLSACertPeriodCode', 'CPC17012', 'Twelve Months', '', '', '1', 0, 'en', CURRENT TIMESTAMP, 1);
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSACalcCertDateRange.calcCertificationDates', 'curam', 'molsa.pd.facade', 'curam.molsa.pd.facade.MOLSACalcCertDateRange.calcCertificationDates', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSACalcCertDateRange.getCertModifiableInd', 'curam', 'molsa.pd.facade', ' curam.molsa.pd.facade.MOLSACalcCertDateRange.getCertModifiableInd', 'Y');
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSACalcCertDateRange.calcCertificationDates', 'FUNCTION', 0);
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSACalcCertDateRange.getCertModifiableInd', 'FUNCTION', 0);
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSACalcCertDateRange.calcCertificationDates', 'MOLSACalcCertDateRange.calcCertificationDates');
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSACalcCertDateRange.getCertModifiableInd', 'MOLSACalcCertDateRange.getCertModifiableInd');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSACalcCertDateRange.calcCertificationDates');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSACalcCertDateRange.getCertModifiableInd');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAExpCertCloseCaseBatch.process', 'curam', 'molsa.pd.batch', 'curam.molsa.pd.batch.MOLSAExpCertCloseCaseBatch.process', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAExpCertCloseCaseBatchStream.process', 'curam', 'molsa.pd.batch', 'curam.molsa.pd.batch.MOLSAExpCertCloseCaseBatchStream.process', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAExpCertSuspendCaseBatch.process', 'curam', 'molsa.pd.batch', 'curam.molsa.pd.batch.MOLSAExpCertSuspendCaseBatch.process', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAExpCertSuspendCaseBatchStream.process', 'curam', 'molsa.pd.batch', 'curam.molsa.pd.batch.MOLSAExpCertSuspendCaseBatchStream.process', 'Y');
+--
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSAExpCertCloseCaseBatch.process', 'FUNCTION', 0);
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSAExpCertCloseCaseBatchStream.process', 'FUNCTION', 0);
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSAExpCertSuspendCaseBatch.process', 'FUNCTION', 0);
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSAExpCertSuspendCaseBatchStream.process', 'FUNCTION', 0);
+--
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSAExpCertCloseCaseBatch.process', 'MOLSAExpCertCloseCaseBatch.process');
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSAExpCertCloseCaseBatchStream.process', 'MOLSAExpCertCloseCaseBatchStream.process');
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSAExpCertSuspendCaseBatch.process', 'MOLSAExpCertSuspendCaseBatch.process');
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSAExpCertSuspendCaseBatchStream.process', 'MOLSAExpCertSuspendCaseBatchStream.process');
+--
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSAExpCertCloseCaseBatch.process');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSAExpCertCloseCaseBatchStream.process');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSAExpCertSuspendCaseBatch.process');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSAExpCertSuspendCaseBatchStream.process');
+--
+INSERT INTO BatchProcDef (ProcessDefName, AppName, ClassName, OpName) values ('MOLSAExpCertCloseCaseBatch', 'curam', 'MOLSAExpCertCloseCaseBatch', 'process');
+INSERT INTO BatchProcDef (ProcessDefName, AppName, ClassName, OpName) values ('MOLSAExpCertCloseCaseBatch', 'curam', 'MOLSAExpCertCloseCaseBatch', 'process');
+INSERT INTO BatchProcDef (ProcessDefName, AppName, ClassName, OpName) values ('MOLSAExpCertCloseCaseBatchStream', 'curam', 'MOLSAExpCertCloseCaseBatchStream', 'process');
+INSERT INTO BatchProcDef (ProcessDefName, AppName, ClassName, OpName) values ('MOLSAExpCertCloseCaseBatchStream', 'curam', 'MOLSAExpCertCloseCaseBatchStream', 'process');
+INSERT INTO BatchParamDef (ProcessDefName, ParamName, ParamType) values ('MOLSAExpCertCloseCaseBatchStream', 'instanceID', 'BATCH_PROCESS_INSTANCE_ID');
+INSERT INTO BatchParamDef (ProcessDefName, ParamName, ParamType) values ('MOLSAExpCertCloseCaseBatchStream', 'processingDate', 'CURAM_DATE');
+INSERT INTO BatchProcDef (ProcessDefName, AppName, ClassName, OpName) values ('MOLSAExpCertSuspendCaseBatch', 'curam', 'MOLSAExpCertSuspendCaseBatch', 'process');
+INSERT INTO BatchProcDef (ProcessDefName, AppName, ClassName, OpName) values ('MOLSAExpCertSuspendCaseBatch', 'curam', 'MOLSAExpCertSuspendCaseBatch', 'process');
+INSERT INTO BatchProcDef (ProcessDefName, AppName, ClassName, OpName) values ('MOLSAExpCertSuspendCaseBatchStream', 'curam', 'MOLSAExpCertSuspendCaseBatchStream', 'process');
+INSERT INTO BatchProcDef (ProcessDefName, AppName, ClassName, OpName) values ('MOLSAExpCertSuspendCaseBatchStream', 'curam', 'MOLSAExpCertSuspendCaseBatchStream', 'process');
+INSERT INTO BatchParamDef (ProcessDefName, ParamName, ParamType) values ('MOLSAExpCertSuspendCaseBatchStream', 'instanceID', 'BATCH_PROCESS_INSTANCE_ID');
+INSERT INTO BatchParamDef (ProcessDefName, ParamName, ParamType) values ('MOLSAExpCertSuspendCaseBatchStream', 'processingDate', 'CURAM_DATE');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+--
+CREATE TABLE MOLSAFINANCIALSCHEDULE(
+MOLSAFINANCIALSCHEDULEID BIGINT not null, 
+RUNDATE DATE, 
+RUNMONTH INT not null, 
+RUNYEAR INT not null, 
+BATCHTYPE CHARACTER(10), 
+BATCHSCHEDULESTATUS CHARACTER(10), 
+VERSIONNO INT not null, 
+LASTWRITTEN TIMESTAMP
+);
+--
+ALTER TABLE MOLSAFINANCIALSCHEDULE ADD
+CONSTRAINT MOLSAFINANCIALSCHEDULE PRIMARY KEY(MOLSAFINANCIALSCHEDULEID);
+--
+ONSTRAINT MOLSAFINANCIALSCHEDULE PRIMARY KEY(MOLSAFINANCIALSCHEDULEID);
+--
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAFinancialScheduleBatch.process', 'curam', 'molsa.financial.batch', 'curam.molsa.financial.batch.MOLSAFinancialScheduleBatch.process', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAFinancialScheduleBatch.process', 'curam', 'molsa.financial.batch', 'curam.molsa.financial.batch.MOLSAFinancialScheduleBatch.process', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAFinancialSchedule.cancelSchedule', 'curam', 'molsa.financial.facade', 'curam.molsa.financial.facade.MOLSAFinancialSchedule.cancelSchedule', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAFinancialSchedule.cancelSchedule', 'curam', 'molsa.financial.facade', 'curam.molsa.financial.facade.MOLSAFinancialSchedule.cancelSchedule', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAFinancialSchedule.completeSchedule', 'curam', 'molsa.financial.facade', 'curam.molsa.financial.facade.MOLSAFinancialSchedule.completeSchedule', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAFinancialSchedule.completeSchedule', 'curam', 'molsa.financial.facade', 'curam.molsa.financial.facade.MOLSAFinancialSchedule.completeSchedule', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAFinancialSchedule.createNewCompletedSchedule', 'curam', 'molsa.financial.facade', 'curam.molsa.financial.facade.MOLSAFinancialSchedule.createNewCompletedSchedule', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAFinancialSchedule.createNewCompletedSchedule', 'curam', 'molsa.financial.facade', 'curam.molsa.financial.facade.MOLSAFinancialSchedule.createNewCompletedSchedule', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAFinancialSchedule.createNewSchedule', 'curam', 'molsa.financial.facade', 'curam.molsa.financial.facade.MOLSAFinancialSchedule.createNewSchedule', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAFinancialSchedule.createNewSchedule', 'curam', 'molsa.financial.facade', 'curam.molsa.financial.facade.MOLSAFinancialSchedule.createNewSchedule', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAFinancialSchedule.getCurrentMonthScheduleByBatchType', 'curam', 'molsa.financial.facade', 'curam.molsa.financial.facade.MOLSAFinancialSchedule.getCurrentMonthScheduleByBatchType', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAFinancialSchedule.getCurrentMonthScheduleByBatchType', 'curam', 'molsa.financial.facade', 'curam.molsa.financial.facade.MOLSAFinancialSchedule.getCurrentMonthScheduleByBatchType', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAFinancialSchedule.listSchedule', 'curam', 'molsa.financial.facade', 'curam.molsa.financial.facade.MOLSAFinancialSchedule.listSchedule', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAFinancialSchedule.listSchedule', 'curam', 'molsa.financial.facade', 'curam.molsa.financial.facade.MOLSAFinancialSchedule.listSchedule', 'Y');
+--
+INSERT INTO BatchProcDef (ProcessDefName, AppName, ClassName, OpName) values ('MOLSAFinancialScheduleBatch', 'curam', 'MOLSAFinancialScheduleBatch', 'process');
+INSERT INTO BatchProcDef (ProcessDefName, AppName, ClassName, OpName) values ('MOLSAFinancialScheduleBatch', 'curam', 'MOLSAFinancialScheduleBatch', 'process');
+--
+INSERT INTO CodeTableHeader (TableName, TimeEntered, DefaultCode, LASTWRITTEN, VERSIONNO) VALUES ('MOLSAFinancialBatchType', CURRENT TIMESTAMP, 'FBT17001', CURRENT TIMESTAMP, 1);
+INSERT INTO CTDISPLAYNAME (TableName, LOCALEIdentifier,TEXT,LASTWRITTEN ) VALUES ( 'MOLSAFinancialBatchType','en','Financial Batch Type', CURRENT TIMESTAMP);
+INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('MOLSAFinancialBatchType', 'FBT17001', 'Main Batch', '', '', '1', 1, 'en', CURRENT TIMESTAMP, 1);
+INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('MOLSAFinancialBatchType', 'FBT17002', 'Mid Batch', '', '', '1', 2, 'en', CURRENT TIMESTAMP, 1);
+--
+INSERT INTO CodeTableHeader (TableName, TimeEntered, DefaultCode, LASTWRITTEN, VERSIONNO) VALUES ('MOLSAFinScheduleStatus', CURRENT TIMESTAMP, 'FBS17001', CURRENT TIMESTAMP, 1);
+INSERT INTO CTDISPLAYNAME (TableName, LOCALEIdentifier,TEXT,LASTWRITTEN ) VALUES ( 'MOLSAFinScheduleStatus','en','Molsa Financial Schedule Status', CURRENT TIMESTAMP);
+INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('MOLSAFinScheduleStatus', 'FBS17001', 'Active', '', '', '1', 1, 'en', CURRENT TIMESTAMP, 1);
+INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('MOLSAFinScheduleStatus', 'FBS17002', 'Canceled', '', '', '1', 2, 'en', CURRENT TIMESTAMP, 1);
+INSERT INTO CodeTableItem (TABLENAME, CODE, DESCRIPTION, ANNOTATION, COMMENTS, ISENABLED, SORTORDER, LOCALEIDENTIFIER, LASTWRITTEN, VERSIONNO) VALUES ('MOLSAFinScheduleStatus', 'FBS17003', 'Executed', '', '', '1', 3, 'en', CURRENT TIMESTAMP, 1);
+--
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSAFinancialSchedule.cancelSchedule', 'FUNCTION', 0);
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSAFinancialSchedule.completeSchedule', 'FUNCTION', 0);
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSAFinancialSchedule.createNewCompletedSchedule', 'FUNCTION', 0);
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSAFinancialSchedule.createNewSchedule', 'FUNCTION', 0);
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSAFinancialSchedule.getCurrentMonthScheduleByBatchType', 'FUNCTION', 0);
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSAFinancialSchedule.listSchedule', 'FUNCTION', 0);
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSAFinancialScheduleBatch.process', 'FUNCTION', 0);
+--
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSAFinancialSchedule.cancelSchedule', 'MOLSAFinancialSchedule.cancelSchedule', CURRENT TIMESTAMP);
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSAFinancialSchedule.completeSchedule', 'MOLSAFinancialSchedule.completeSchedule', CURRENT TIMESTAMP);
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSAFinancialSchedule.createNewCompletedSchedule', 'MOLSAFinancialSchedule.createNewCompletedSchedule', CURRENT TIMESTAMP);
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSAFinancialSchedule.createNewSchedule', 'MOLSAFinancialSchedule.createNewSchedule', CURRENT TIMESTAMP);
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSAFinancialSchedule.getCurrentMonthScheduleByBatchType', 'MOLSAFinancialSchedule.getCurrentMonthScheduleByBatchType', CURRENT TIMESTAMP);
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSAFinancialSchedule.listSchedule', 'MOLSAFinancialSchedule.listSchedule', CURRENT TIMESTAMP);
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSAFinancialScheduleBatch.process', 'MOLSAFinancialScheduleBatch.process', CURRENT TIMESTAMP);
+--
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSAFinancialSchedule.cancelSchedule');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSAFinancialSchedule.completeSchedule');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSAFinancialSchedule.createNewCompletedSchedule');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSAFinancialSchedule.createNewSchedule');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSAFinancialSchedule.getCurrentMonthScheduleByBatchType');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSAFinancialSchedule.listSchedule');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSAFinancialScheduleBatch.process');
+--
+</t>
+  </si>
+  <si>
+    <t>CR 7.2 Financial batches should run more securely</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modified Existing files
+-----------------------
+\EJBServer\components\MOLSA\clientapps\MolsaManagerAppViews\MOLSAMAPPWorkspaceSection.sec  
+\EJBServer\components\MOLSA\clientapps\MolsaManagerAppViews\MOLSAMAPPWorkspaceSectionShortcuts.properties  
+\EJBServer\components\MOLSA\clientapps\MolsaManagerAppViews\MOLSAMAPPWorkspaceSectionShortcuts.ssp  
+\EJBServer\components\MOLSA\properties\Application.prx 
+\EJBServer\components\MOLSA_ar\clientapps\MolsaManagerAppViews\MOLSAMAPPWorkspaceSection.sec  
+\EJBServer\components\MOLSA_ar\clientapps\MolsaManagerAppViews\MOLSAMAPPWorkspaceSectionShortcuts.ssp  
+Added New file and folders
+--------------------------
+\EJBServer\components\MOLSA\clientapps\MOLSAFinancialScheduleList.properties  
+\EJBServer\components\MOLSA\clientapps\MOLSAFinancialScheduleList.tab  
+\EJBServer\components\MOLSA\codetable\CT_MOLSAFinScheduleStatus.ctx  
+\EJBServer\components\MOLSA\codetable\CT_MOLSAFinancialBatchType.ctx  
+\EJBServer\components\MOLSA\message\MOLSABpoFinancialSchedule.xml  
+\EJBServer\components\MOLSA\model\Packages\Financial\Batch  
+\EJBServer\components\MOLSA\model\Packages\Financial\Batch\Batch.efx  
+\EJBServer\components\MOLSA\model\Packages\Financial\Domain Definition  
+\EJBServer\components\MOLSA\model\Packages\Financial\Domain Definition\DomainDefinition.efx  
+\EJBServer\components\MOLSA\model\Packages\Financial\Entity  
+\EJBServer\components\MOLSA\model\Packages\Financial\Entity\Entity.efx  
+\EJBServer\components\MOLSA\model\Packages\Financial\Facade  
+\EJBServer\components\MOLSA\model\Packages\Financial\Facade\Facade.efx  
+\EJBServer\components\MOLSA\model\Packages\Financial\Financial.efx  
+\EJBServer\components\MOLSA\model\Packages\Financial\ServiceLayer  
+\EJBServer\components\MOLSA\model\Packages\Financial\ServiceLayer\ServiceLayer.efx  
+\EJBServer\components\MOLSA\source\curam\molsa\financial  
+\EJBServer\components\MOLSA\source\curam\molsa\financial\batch  
+\EJBServer\components\MOLSA\source\curam\molsa\financial\batch\impl  
+\EJBServer\components\MOLSA\source\curam\molsa\financial\batch\impl\MOLSAFinancialScheduleBatch.java  
+\EJBServer\components\MOLSA\source\curam\molsa\financial\facade  
+\EJBServer\components\MOLSA\source\curam\molsa\financial\facade\impl  
+\EJBServer\components\MOLSA\source\curam\molsa\financial\facade\impl\MOLSAFinancialSchedule.java  
+\EJBServer\components\MOLSA\source\curam\molsa\financial\sl  
+\EJBServer\components\MOLSA\source\curam\molsa\financial\sl\impl  
+\EJBServer\components\MOLSA\source\curam\molsa\financial\sl\impl\MOLSAMaintainFinancialSchedule.java
+\EJBServer\MOLSA Financial Batch Schedule Execution.bat
+\webclient\components\MOLSA\Financial  
+\webclient\components\MOLSA\Financial\MOLSA_cancelFinancialSchedule.properties  
+\webclient\components\MOLSA\Financial\MOLSA_cancelFinancialSchedule.uim  
+\webclient\components\MOLSA\Financial\MOLSA_createNewFinancialSchedule.properties  
+\webclient\components\MOLSA\Financial\MOLSA_createNewFinancialSchedule.uim  
+\webclient\components\MOLSA\Financial\MOLSA_listFinancialSchedule.properties  
+\webclient\components\MOLSA\Financial\MOLSA_listFinancialSchedule.uim </t>
   </si>
 </sst>
 </file>
@@ -560,9 +714,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,7 +783,7 @@
       </c>
       <c r="G3" s="1"/>
       <c r="I3" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -637,10 +791,10 @@
         <v>42787</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -649,15 +803,31 @@
         <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="397.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="1"/>
-      <c r="G5" s="1"/>
+    <row r="5" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>42797</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C6" s="4"/>
@@ -692,22 +862,53 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
-      <Description>UQKZYU5EZKJQ-17-950</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -895,53 +1096,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
+      <Description>UQKZYU5EZKJQ-17-950</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -954,18 +1124,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1926F8BC-3749-487B-86BA-515B8CAD861D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e967487d-3eea-483d-b969-e50e6c114ffa"/>
-    <ds:schemaRef ds:uri="43475cab-d89f-451e-a1e3-4db005e0f558"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -990,9 +1151,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1926F8BC-3749-487B-86BA-515B8CAD861D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e967487d-3eea-483d-b969-e50e6c114ffa"/>
+    <ds:schemaRef ds:uri="43475cab-d89f-451e-a1e3-4db005e0f558"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added details for CR1.1
</commit_message>
<xml_diff>
--- a/Development/Artifacts/Changes from CR Mar 2017.xlsx
+++ b/Development/Artifacts/Changes from CR Mar 2017.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="02-21-2017" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Bugzilla Ticket No</t>
   </si>
@@ -281,6 +281,25 @@
 \webclient\components\MOLSA\Financial\MOLSA_createNewFinancialSchedule.uim  
 \webclient\components\MOLSA\Financial\MOLSA_listFinancialSchedule.properties  
 \webclient\components\MOLSA\Financial\MOLSA_listFinancialSchedule.uim </t>
+  </si>
+  <si>
+    <t>March 5,2017</t>
+  </si>
+  <si>
+    <t>INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSACommunicationDA.listTemplateByTypeAndParticipantAutoDisplay', 'curam', 'molsa.core.facade', 'curam.molsa.core.facade.impl.MOLSACommunicationDA.listTemplateByTypeAndParticipantAutoDisplay', 'Y');
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, '2017-03-05 03:42:25', 'MOLSACommunicationDA.listTemplateByTypeAndParticipantAutoDisplay', 'FUNCTION', 0);
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME) VALUES ('MOLSACommunicationDA.listTemplateByTypeAndParticipantAutoDisplay','MOLSACommunicationDA.listTemplateByTypeAndParticipantAutoDisplay');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSACommunicationDA.listTemplateByTypeAndParticipantAutoDisplay');</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/EJBServer/components/MOLSA/model/Packages/Reference Model/Facade/Communication.efx
+</t>
+  </si>
+  <si>
+    <t>CR1.1 Diplaying the list of Proforma(Letters) without search, while creating</t>
   </si>
 </sst>
 </file>
@@ -468,7 +487,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -503,7 +522,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -715,23 +734,23 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="136" customWidth="1"/>
-    <col min="4" max="4" width="35.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="187.88671875" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" customWidth="1"/>
-    <col min="9" max="9" width="53.109375" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="187.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="53.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -760,12 +779,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
       <c r="G2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="124.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>42781</v>
       </c>
@@ -786,7 +805,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="408.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>42787</v>
       </c>
@@ -829,24 +848,41 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C6" s="4"/>
+    <row r="6" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="I10" s="1"/>
     </row>
@@ -863,55 +899,33 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
+      <Description>UQKZYU5EZKJQ-17-950</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003520CC91E1C90A4F9689A135D663C63F" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5bea9beecb72e899f05172e22af69af0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e967487d-3eea-483d-b969-e50e6c114ffa" xmlns:ns3="43475cab-d89f-451e-a1e3-4db005e0f558" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="438d5435a0413bb8242127eebe6f163c" ns2:_="" ns3:_="">
     <xsd:import namespace="e967487d-3eea-483d-b969-e50e6c114ffa"/>
@@ -1095,43 +1109,82 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
-      <Description>UQKZYU5EZKJQ-17-950</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1926F8BC-3749-487B-86BA-515B8CAD861D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e967487d-3eea-483d-b969-e50e6c114ffa"/>
+    <ds:schemaRef ds:uri="43475cab-d89f-451e-a1e3-4db005e0f558"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0051AA5-43D6-41A0-9086-D5D3DFF72221}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1150,27 +1203,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1926F8BC-3749-487B-86BA-515B8CAD861D}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e967487d-3eea-483d-b969-e50e6c114ffa"/>
-    <ds:schemaRef ds:uri="43475cab-d89f-451e-a1e3-4db005e0f558"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Bhaskar CR # 2.2 Cases to be renewed should create a task to the caseworker 45 days before the end of certification date.
</commit_message>
<xml_diff>
--- a/Development/Artifacts/Changes from CR Mar 2017.xlsx
+++ b/Development/Artifacts/Changes from CR Mar 2017.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Bugzilla Ticket No</t>
   </si>
@@ -300,6 +300,49 @@
   </si>
   <si>
     <t>CR1.1 Diplaying the list of Proforma(Letters) without search, while creating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR 2.2 Cases to be renewed should create a task to the caseworker 45 days before the end of certification date. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">New files:
+\EJBServer\components\MOLSA\source\curam\molsa\pd\batch\impl\MOLSACertificationExpiryBatch.java  
+\EJBServer\components\MOLSA\source\curam\molsa\pd\batch\impl\MOLSACertificationExpiryBatchStream.java  
+\EJBServer\components\MOLSA\source\curam\molsa\pd\batch\impl\MOLSACertificationExpiryBatchStreamWrapper.java  
+\EJBServer\components\MOLSA\source\curam\molsa\pd\batch\impl\MOLSACertificationExpiryBatchWrapper.java  
+\EJBServer\components\MOLSA\workflow\MOLSACertificationExpiryTask_v1.xml 
+Modified Files: 
+\EJBServer\components\MOLSA\codetable\CT_BatchProcessName.ctx  
+\EJBServer\components\MOLSA\data\initial\ALLOCATIONTARGET.dmx  
+\EJBServer\components\MOLSA\data\initial\ALLOCATIONTARGETITEM.dmx  
+\EJBServer\components\MOLSA\data\initial\WORKQUEUE.dmx  
+\EJBServer\components\MOLSA\model\Packages\ProductDelivery\Certification\Batch.efx  
+\EJBServer\components\MOLSA\properties\Application.prx  
+\EJBServer\components\MOLSA\source\curam\molsa\constants\impl\MOLSAConstants.java </t>
+  </si>
+  <si>
+    <t>INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSACertificationExpiryBatch.process', 'curam', 'molsa.pd.batch', 'curam.molsa.pd.batch.MOLSACertificationExpiryBatch.process', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSACertificationExpiryBatchStream.process', 'curam', 'molsa.pd.batch', 'curam.molsa.pd.batch.MOLSACertificationExpiryBatchStream.process', 'Y');
+--
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSACertificationExpiryBatch.process', 'FUNCTION', 0);
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, null, 'MOLSACertificationExpiryBatchStream.process', 'FUNCTION', 0);
+--
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSACertificationExpiryBatch.process', 'MOLSACertificationExpiryBatch.process');
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSACertificationExpiryBatchStream.process', 'MOLSACertificationExpiryBatchStream.process');
+--
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSACertificationExpiryBatch.process');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSACertificationExpiryBatchStream.process');
+--
+INSERT INTO BatchProcDef (ProcessDefName, AppName, ClassName, OpName) values ('MOLSACertificationExpiryBatch', 'curam', 'MOLSACertificationExpiryBatch', 'process');
+INSERT INTO BatchProcDef (ProcessDefName, AppName, ClassName, OpName) values ('MOLSACertificationExpiryBatchStream', 'curam', 'MOLSACertificationExpiryBatchStream', 'process');
+INSERT INTO BatchParamDef (ProcessDefName, ParamName, ParamType) values ('MOLSACertificationExpiryBatchStream', 'instanceID', 'BATCH_PROCESS_INSTANCE_ID');
+INSERT INTO BatchParamDef (ProcessDefName, ParamName, ParamType) values ('MOLSACertificationExpiryBatchStream', 'processingDate', 'CURAM_DATE');
+--
+INSERT INTO WORKQUEUE (ADMINISTRATORUSERNAME, ALLOWUSERSUBSCRIPTIONIND, COMMENTS, LASTWRITTEN, NAME, SENSITIVITY, UPPERNAME, VERSIONNO, WORKQUEUEID) VALUES ('admin', '1', 'This work queue is used to assign tasks to case workers when the PD certification is going to expired in 45 days.', '2001-01-01 00:00:00', 'MOLSACertExpiryQueue', '0', 'MOLSACERTEXPIRY', 1, 45014);
+--
+INSERT INTO ALLOCATIONTARGET (ALLOCATIONTARGETID, COMMENTS, NAME) VALUES ('MOLSACertExpiryQueue', 'MOLSA Certification Expiry Queue', 'MOLSACertExpiryQueue');
+--
+INSERT INTO ALLOCATIONTARGETITEM (ALLOCATIONTARGETID, ALLOCATIONTARGETITEMID, RELATEDID, RELATEDNAME, TYPE) VALUES ('MOLSACertExpiryQueue', 45006, 45014, 'MOLSACertExpiryQueue', 'RL23');</t>
   </si>
 </sst>
 </file>
@@ -376,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -389,9 +432,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -487,7 +527,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -522,7 +562,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -735,12 +775,12 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="136" customWidth="1"/>
     <col min="4" max="4" width="35.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
@@ -751,7 +791,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="43.15" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -785,7 +825,7 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="124.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>42781</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -801,12 +841,12 @@
         <v>9</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="408.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>42787</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -824,12 +864,12 @@
       <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>42797</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -849,7 +889,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -869,10 +909,26 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="390" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>42807</v>
+      </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="G7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
@@ -898,34 +954,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
-      <Description>UQKZYU5EZKJQ-17-950</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003520CC91E1C90A4F9689A135D663C63F" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5bea9beecb72e899f05172e22af69af0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e967487d-3eea-483d-b969-e50e6c114ffa" xmlns:ns3="43475cab-d89f-451e-a1e3-4db005e0f558" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="438d5435a0413bb8242127eebe6f163c" ns2:_="" ns3:_="">
     <xsd:import namespace="e967487d-3eea-483d-b969-e50e6c114ffa"/>
@@ -1109,6 +1137,34 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
+      <Description>UQKZYU5EZKJQ-17-950</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
@@ -1160,9 +1216,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0051AA5-43D6-41A0-9086-D5D3DFF72221}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e967487d-3eea-483d-b969-e50e6c114ffa"/>
+    <ds:schemaRef ds:uri="43475cab-d89f-451e-a1e3-4db005e0f558"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1185,20 +1252,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0051AA5-43D6-41A0-9086-D5D3DFF72221}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e967487d-3eea-483d-b969-e50e6c114ffa"/>
-    <ds:schemaRef ds:uri="43475cab-d89f-451e-a1e3-4db005e0f558"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Bhaskar - CR # 8.5 Person Search Page Changes
</commit_message>
<xml_diff>
--- a/Development/Artifacts/Changes from CR Mar 2017.xlsx
+++ b/Development/Artifacts/Changes from CR Mar 2017.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="02-21-2017" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Bugzilla Ticket No</t>
   </si>
@@ -343,6 +343,27 @@
 INSERT INTO ALLOCATIONTARGET (ALLOCATIONTARGETID, COMMENTS, NAME) VALUES ('MOLSACertExpiryQueue', 'MOLSA Certification Expiry Queue', 'MOLSACertExpiryQueue');
 --
 INSERT INTO ALLOCATIONTARGETITEM (ALLOCATIONTARGETID, ALLOCATIONTARGETITEMID, RELATEDID, RELATEDNAME, TYPE) VALUES ('MOLSACertExpiryQueue', 45006, 45014, 'MOLSACertExpiryQueue', 'RL23');</t>
+  </si>
+  <si>
+    <t>CR 8.5 Person Search Page Changes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Files Added:
+\webclient\components\MOLSA\ReferenceApp\core\Person\Search\MOLSAPerson_searchCriteriaView.properties
+\webclient\components\MOLSA\ReferenceApp\core\Person\Search\MOLSAPerson_searchCriteriaView.vim
+\webclient\components\MOLSA_ar\ReferenceApp\core\Person\Search\MOLSAPerson_searchCriteriaView_ar.properties
+\EJBServer\components\MOLSA\message\MOLSABpoPersonSearch.xml
+\EJBServer\components\MOLSA\source\curam\molsa\core\impl\MOLSADatabasePersonSearch.java 
+Existing Files Mofified:
+\webclient\components\MOLSA\ReferenceApp\core\Person\Search\Person_search1.uim  
+\EJBServer\components\MOLSA\model\Packages\Reference Model\Core.efx  
+\EJBServer\components\MOLSA\model\Packages\Reference Model\Facade\Person.efx  
+\EJBServer\components\MOLSA\model\Packages\Reference Model\Facade.efx  
+\EJBServer\components\MOLSA\model\Packages\Reference Model\Person Search\Person Search.efx  
+\EJBServer\components\MOLSA\source\curam\molsa\core\facade\impl\MOLSAPersonDA.java  </t>
   </si>
 </sst>
 </file>
@@ -775,22 +796,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="136" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="187.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="53.140625" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="187.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" customWidth="1"/>
+    <col min="9" max="9" width="53.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
@@ -819,12 +840,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
       <c r="G2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="124.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>42781</v>
       </c>
@@ -845,7 +866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="408.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>42787</v>
       </c>
@@ -888,7 +909,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
@@ -909,7 +930,7 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="390" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="360" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>42807</v>
       </c>
@@ -930,15 +951,29 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
+    <row r="8" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>42811</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
       <c r="I10" s="1"/>
     </row>
@@ -954,6 +989,34 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
+      <Description>UQKZYU5EZKJQ-17-950</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003520CC91E1C90A4F9689A135D663C63F" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5bea9beecb72e899f05172e22af69af0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e967487d-3eea-483d-b969-e50e6c114ffa" xmlns:ns3="43475cab-d89f-451e-a1e3-4db005e0f558" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="438d5435a0413bb8242127eebe6f163c" ns2:_="" ns3:_="">
     <xsd:import namespace="e967487d-3eea-483d-b969-e50e6c114ffa"/>
@@ -1137,34 +1200,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
-      <Description>UQKZYU5EZKJQ-17-950</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
@@ -1216,20 +1251,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0051AA5-43D6-41A0-9086-D5D3DFF72221}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e967487d-3eea-483d-b969-e50e6c114ffa"/>
-    <ds:schemaRef ds:uri="43475cab-d89f-451e-a1e3-4db005e0f558"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1252,9 +1276,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0051AA5-43D6-41A0-9086-D5D3DFF72221}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e967487d-3eea-483d-b969-e50e6c114ffa"/>
+    <ds:schemaRef ds:uri="43475cab-d89f-451e-a1e3-4db005e0f558"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>